<commit_message>
site updated with new data
</commit_message>
<xml_diff>
--- a/data/GIAD_status_goal.xlsx
+++ b/data/GIAD_status_goal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/aaron_pilot_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D669CEBB-E2D6-4B49-9C67-FAEDBCBF4944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2166052-E1B5-5B44-974F-8F0147CCF124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14280" yWindow="-19560" windowWidth="28800" windowHeight="16160" xr2:uid="{87C20961-A433-BF4D-865D-2FAA4F538231}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{87C20961-A433-BF4D-865D-2FAA4F538231}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,10 +429,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>89.81</v>
+        <v>88.68</v>
       </c>
       <c r="D2">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -451,10 +451,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>87.32</v>
+        <v>87.5</v>
       </c>
       <c r="D4">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -473,10 +473,10 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>88.94</v>
+        <v>88.1</v>
       </c>
       <c r="E6">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -484,7 +484,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>85.94</v>
+        <v>85.84</v>
       </c>
       <c r="E7">
         <v>226</v>
@@ -495,10 +495,10 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>95.09</v>
+        <v>92</v>
       </c>
       <c r="E8">
-        <v>265</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>